<commit_message>
example: better structure of exp_02
</commit_message>
<xml_diff>
--- a/example/game_02_click_cookies/artifacts.xlsx
+++ b/example/game_02_click_cookies/artifacts.xlsx
@@ -518,13 +518,13 @@
         <v>globalMultiplier</v>
       </c>
       <c r="G4">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="H4">
         <v>30</v>
       </c>
       <c r="I4" t="str">
-        <v>所有 CPS 乘以 1.5。</v>
+        <v>所有 CPS 乘以 1.6。</v>
       </c>
       <c r="J4" t="str">
         <v>https://cdn.jsdelivr.net/gh/twitter/twemoji@14.0.2/assets/72x72/1f9b5.png</v>
@@ -550,13 +550,13 @@
         <v>clickMultiplier</v>
       </c>
       <c r="G5">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="H5">
         <v>25</v>
       </c>
       <c r="I5" t="str">
-        <v>点击产量加倍并更快上浮。</v>
+        <v>点击产量翻至 3 倍，并更快上浮。</v>
       </c>
       <c r="J5" t="str">
         <v>https://cdn.jsdelivr.net/gh/twitter/twemoji@14.0.2/assets/72x72/1f36c.png</v>
@@ -614,13 +614,13 @@
         <v>producerBoost:60000005</v>
       </c>
       <c r="G7">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="H7">
         <v>45</v>
       </c>
       <c r="I7" t="str">
-        <v>工厂生产效率提升 150%。</v>
+        <v>工厂生产效率提升 200%。</v>
       </c>
       <c r="J7" t="str">
         <v>https://cdn.jsdelivr.net/gh/twitter/twemoji@14.0.2/assets/72x72/23f1.png</v>
@@ -646,13 +646,13 @@
         <v>cpsAdditive</v>
       </c>
       <c r="G8">
-        <v>200</v>
+        <v>50000</v>
       </c>
       <c r="H8">
         <v>40</v>
       </c>
       <c r="I8" t="str">
-        <v>额外 +200 CPS。</v>
+        <v>额外 +50,000 CPS。</v>
       </c>
       <c r="J8" t="str">
         <v>https://cdn.jsdelivr.net/gh/twitter/twemoji@14.0.2/assets/72x72/23f3.png</v>

</xml_diff>

<commit_message>
feat(example): diversify click-cookies artifacts
</commit_message>
<xml_diff>
--- a/example/game_02_click_cookies/artifacts.xlsx
+++ b/example/game_02_click_cookies/artifacts.xlsx
@@ -576,22 +576,22 @@
         <v>3</v>
       </c>
       <c r="E6" t="str">
-        <v>Grandma Covenant</v>
+        <v>Pocket Chronometer</v>
       </c>
       <c r="F6" t="str">
-        <v>producerBoost:60000002</v>
+        <v>offlineMultiplier</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H6">
         <v>35</v>
       </c>
       <c r="I6" t="str">
-        <v>奶奶建筑产出 *3。</v>
+        <v>离线收益翻倍，归来即可收割。</v>
       </c>
       <c r="J6" t="str">
-        <v>https://cdn.jsdelivr.net/gh/twitter/twemoji@14.0.2/assets/72x72/1f465.png</v>
+        <v>https://cdn.jsdelivr.net/gh/twitter/twemoji@14.0.2/assets/72x72/23f1.png</v>
       </c>
     </row>
     <row r="7">
@@ -608,22 +608,22 @@
         <v>4</v>
       </c>
       <c r="E7" t="str">
-        <v>Factory Time Dilation</v>
+        <v>Quantum Ledger</v>
       </c>
       <c r="F7" t="str">
-        <v>producerBoost:60000005</v>
+        <v>costReduction</v>
       </c>
       <c r="G7">
-        <v>3</v>
+        <v>0.15</v>
       </c>
       <c r="H7">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="I7" t="str">
-        <v>工厂生产效率提升 200%。</v>
+        <v>所有建筑成本降低 15%。</v>
       </c>
       <c r="J7" t="str">
-        <v>https://cdn.jsdelivr.net/gh/twitter/twemoji@14.0.2/assets/72x72/23f1.png</v>
+        <v>https://cdn.jsdelivr.net/gh/twitter/twemoji@14.0.2/assets/72x72/1f4b0.png</v>
       </c>
     </row>
     <row r="8">
@@ -640,22 +640,22 @@
         <v>5</v>
       </c>
       <c r="E8" t="str">
-        <v>Chrono Crumbs</v>
+        <v>Starfarer Compass</v>
       </c>
       <c r="F8" t="str">
-        <v>cpsAdditive</v>
+        <v>prestigeBonus</v>
       </c>
       <c r="G8">
-        <v>50000</v>
+        <v>0.25</v>
       </c>
       <c r="H8">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="I8" t="str">
-        <v>额外 +50,000 CPS。</v>
+        <v>声望重置额外 +25% 神器点。</v>
       </c>
       <c r="J8" t="str">
-        <v>https://cdn.jsdelivr.net/gh/twitter/twemoji@14.0.2/assets/72x72/23f3.png</v>
+        <v>https://cdn.jsdelivr.net/gh/twitter/twemoji@14.0.2/assets/72x72/1f320.png</v>
       </c>
     </row>
   </sheetData>

</xml_diff>